<commit_message>
Files auto-saved. Need to commit to pull
</commit_message>
<xml_diff>
--- a/data/clean_data/Oil Consumption - Barrels-YearFixed.xlsx
+++ b/data/clean_data/Oil Consumption - Barrels-YearFixed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\homework\FinalProject\Final_Team_Project\data\clean_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FAA443-E5A4-4E6F-9E4D-4DA37FEAB175}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F122CB-1EFA-45D5-AA6C-B991117B64DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B05CE6E3-9926-4D82-BA16-B6FEB14B547A}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3687" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3742" uniqueCount="71">
   <si>
     <t>Canada</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>Total Africa</t>
+  </si>
+  <si>
+    <t>Total Middle East</t>
   </si>
 </sst>
 </file>
@@ -663,10 +666,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C3685"/>
+  <dimension ref="A1:C3740"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3162" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3606" sqref="G3606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -40548,8 +40551,613 @@
       <c r="B3685" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3685" s="4">
+      <c r="C3685" s="3">
         <v>355.76715360614571</v>
+      </c>
+    </row>
+    <row r="3686" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3686" s="9">
+        <v>23743</v>
+      </c>
+      <c r="B3686" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3686" s="3">
+        <v>870.00565430442828</v>
+      </c>
+    </row>
+    <row r="3687" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3687" s="9">
+        <v>24108</v>
+      </c>
+      <c r="B3687" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3687" s="3">
+        <v>894.34242038045772</v>
+      </c>
+    </row>
+    <row r="3688" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3688" s="9">
+        <v>24473</v>
+      </c>
+      <c r="B3688" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3688" s="3">
+        <v>922.96024422263201</v>
+      </c>
+    </row>
+    <row r="3689" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3689" s="9">
+        <v>24838</v>
+      </c>
+      <c r="B3689" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3689" s="3">
+        <v>951.04871811327439</v>
+      </c>
+    </row>
+    <row r="3690" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3690" s="9">
+        <v>25204</v>
+      </c>
+      <c r="B3690" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3690" s="3">
+        <v>984.84839092177651</v>
+      </c>
+    </row>
+    <row r="3691" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3691" s="9">
+        <v>25569</v>
+      </c>
+      <c r="B3691" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3691" s="3">
+        <v>1043.988224157825</v>
+      </c>
+    </row>
+    <row r="3692" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3692" s="9">
+        <v>25934</v>
+      </c>
+      <c r="B3692" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3692" s="3">
+        <v>1098.2894873142525</v>
+      </c>
+    </row>
+    <row r="3693" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3693" s="9">
+        <v>26299</v>
+      </c>
+      <c r="B3693" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3693" s="3">
+        <v>1180.1757072236194</v>
+      </c>
+    </row>
+    <row r="3694" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3694" s="9">
+        <v>26665</v>
+      </c>
+      <c r="B3694" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3694" s="3">
+        <v>1275.9133848665967</v>
+      </c>
+    </row>
+    <row r="3695" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3695" s="9">
+        <v>27030</v>
+      </c>
+      <c r="B3695" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3695" s="3">
+        <v>1360.6817723152933</v>
+      </c>
+    </row>
+    <row r="3696" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3696" s="9">
+        <v>27395</v>
+      </c>
+      <c r="B3696" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3696" s="3">
+        <v>1316.562310673876</v>
+      </c>
+    </row>
+    <row r="3697" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3697" s="9">
+        <v>27760</v>
+      </c>
+      <c r="B3697" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3697" s="3">
+        <v>1501.6015211992765</v>
+      </c>
+    </row>
+    <row r="3698" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3698" s="9">
+        <v>28126</v>
+      </c>
+      <c r="B3698" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3698" s="3">
+        <v>1706.1689259447928</v>
+      </c>
+    </row>
+    <row r="3699" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3699" s="9">
+        <v>28491</v>
+      </c>
+      <c r="B3699" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3699" s="3">
+        <v>1775.7926117267871</v>
+      </c>
+    </row>
+    <row r="3700" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3700" s="9">
+        <v>28856</v>
+      </c>
+      <c r="B3700" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3700" s="3">
+        <v>2018.3628073514913</v>
+      </c>
+    </row>
+    <row r="3701" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3701" s="9">
+        <v>29221</v>
+      </c>
+      <c r="B3701" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3701" s="3">
+        <v>1932.9859880279</v>
+      </c>
+    </row>
+    <row r="3702" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3702" s="9">
+        <v>29587</v>
+      </c>
+      <c r="B3702" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3702" s="3">
+        <v>2116.0385322137345</v>
+      </c>
+    </row>
+    <row r="3703" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3703" s="9">
+        <v>29952</v>
+      </c>
+      <c r="B3703" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3703" s="3">
+        <v>2326.6001881268066</v>
+      </c>
+    </row>
+    <row r="3704" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3704" s="9">
+        <v>30317</v>
+      </c>
+      <c r="B3704" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3704" s="3">
+        <v>2596.5719630330454</v>
+      </c>
+    </row>
+    <row r="3705" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3705" s="9">
+        <v>30682</v>
+      </c>
+      <c r="B3705" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3705" s="3">
+        <v>2832.5710500737168</v>
+      </c>
+    </row>
+    <row r="3706" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3706" s="9">
+        <v>31048</v>
+      </c>
+      <c r="B3706" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3706" s="3">
+        <v>3011.699452196151</v>
+      </c>
+    </row>
+    <row r="3707" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3707" s="9">
+        <v>31413</v>
+      </c>
+      <c r="B3707" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3707" s="3">
+        <v>3001.094099927795</v>
+      </c>
+    </row>
+    <row r="3708" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3708" s="9">
+        <v>31778</v>
+      </c>
+      <c r="B3708" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3708" s="3">
+        <v>3177.4474363134436</v>
+      </c>
+    </row>
+    <row r="3709" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3709" s="9">
+        <v>32143</v>
+      </c>
+      <c r="B3709" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3709" s="3">
+        <v>3309.8131328694667</v>
+      </c>
+    </row>
+    <row r="3710" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3710" s="9">
+        <v>32509</v>
+      </c>
+      <c r="B3710" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3710" s="3">
+        <v>3420.1642871238005</v>
+      </c>
+    </row>
+    <row r="3711" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3711" s="9">
+        <v>32874</v>
+      </c>
+      <c r="B3711" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3711" s="3">
+        <v>3488.553870355991</v>
+      </c>
+    </row>
+    <row r="3712" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3712" s="9">
+        <v>33239</v>
+      </c>
+      <c r="B3712" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3712" s="3">
+        <v>3645.58084058739</v>
+      </c>
+    </row>
+    <row r="3713" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3713" s="9">
+        <v>33604</v>
+      </c>
+      <c r="B3713" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3713" s="3">
+        <v>3851.3607971844503</v>
+      </c>
+    </row>
+    <row r="3714" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3714" s="9">
+        <v>33970</v>
+      </c>
+      <c r="B3714" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3714" s="3">
+        <v>4144.7359845345363</v>
+      </c>
+    </row>
+    <row r="3715" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3715" s="9">
+        <v>34335</v>
+      </c>
+      <c r="B3715" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3715" s="3">
+        <v>4584.5956762283886</v>
+      </c>
+    </row>
+    <row r="3716" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3716" s="9">
+        <v>34700</v>
+      </c>
+      <c r="B3716" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3716" s="3">
+        <v>4600.6411443177631</v>
+      </c>
+    </row>
+    <row r="3717" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3717" s="9">
+        <v>35065</v>
+      </c>
+      <c r="B3717" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3717" s="3">
+        <v>4718.6095407627363</v>
+      </c>
+    </row>
+    <row r="3718" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3718" s="9">
+        <v>35431</v>
+      </c>
+      <c r="B3718" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3718" s="3">
+        <v>4951.4200096755021</v>
+      </c>
+    </row>
+    <row r="3719" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3719" s="9">
+        <v>35796</v>
+      </c>
+      <c r="B3719" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3719" s="3">
+        <v>4861.9457530819218</v>
+      </c>
+    </row>
+    <row r="3720" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3720" s="9">
+        <v>36161</v>
+      </c>
+      <c r="B3720" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3720" s="3">
+        <v>4852.9825312957773</v>
+      </c>
+    </row>
+    <row r="3721" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3721" s="9">
+        <v>36526</v>
+      </c>
+      <c r="B3721" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3721" s="3">
+        <v>5087.4057996598694</v>
+      </c>
+    </row>
+    <row r="3722" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3722" s="9">
+        <v>36892</v>
+      </c>
+      <c r="B3722" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3722" s="3">
+        <v>5320.2230878241608</v>
+      </c>
+    </row>
+    <row r="3723" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3723" s="9">
+        <v>37257</v>
+      </c>
+      <c r="B3723" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3723" s="3">
+        <v>5455.5655945716799</v>
+      </c>
+    </row>
+    <row r="3724" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3724" s="9">
+        <v>37622</v>
+      </c>
+      <c r="B3724" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3724" s="3">
+        <v>5673.7081739788628</v>
+      </c>
+    </row>
+    <row r="3725" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3725" s="9">
+        <v>37987</v>
+      </c>
+      <c r="B3725" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3725" s="3">
+        <v>5997.9598858199779</v>
+      </c>
+    </row>
+    <row r="3726" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3726" s="9">
+        <v>38353</v>
+      </c>
+      <c r="B3726" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3726" s="3">
+        <v>6452.0073769819637</v>
+      </c>
+    </row>
+    <row r="3727" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3727" s="9">
+        <v>38718</v>
+      </c>
+      <c r="B3727" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3727" s="3">
+        <v>6721.9990333413016</v>
+      </c>
+    </row>
+    <row r="3728" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3728" s="9">
+        <v>39083</v>
+      </c>
+      <c r="B3728" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3728" s="3">
+        <v>6972.7757976428093</v>
+      </c>
+    </row>
+    <row r="3729" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3729" s="9">
+        <v>39448</v>
+      </c>
+      <c r="B3729" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3729" s="3">
+        <v>7391.2971528604439</v>
+      </c>
+    </row>
+    <row r="3730" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3730" s="9">
+        <v>39814</v>
+      </c>
+      <c r="B3730" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3730" s="3">
+        <v>7730.3820363724099</v>
+      </c>
+    </row>
+    <row r="3731" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3731" s="9">
+        <v>40179</v>
+      </c>
+      <c r="B3731" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3731" s="3">
+        <v>7987.0544942342603</v>
+      </c>
+    </row>
+    <row r="3732" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3732" s="9">
+        <v>40544</v>
+      </c>
+      <c r="B3732" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3732" s="3">
+        <v>8292.6553892270822</v>
+      </c>
+    </row>
+    <row r="3733" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3733" s="9">
+        <v>40909</v>
+      </c>
+      <c r="B3733" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3733" s="3">
+        <v>8641.9797228655261</v>
+      </c>
+    </row>
+    <row r="3734" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3734" s="9">
+        <v>41275</v>
+      </c>
+      <c r="B3734" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3734" s="3">
+        <v>8867.9129499334595</v>
+      </c>
+    </row>
+    <row r="3735" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3735" s="9">
+        <v>41640</v>
+      </c>
+      <c r="B3735" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3735" s="3">
+        <v>8993.0580440155791</v>
+      </c>
+    </row>
+    <row r="3736" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3736" s="9">
+        <v>42005</v>
+      </c>
+      <c r="B3736" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3736" s="3">
+        <v>8987.209124027524</v>
+      </c>
+    </row>
+    <row r="3737" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3737" s="9">
+        <v>42370</v>
+      </c>
+      <c r="B3737" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3737" s="3">
+        <v>9190.6470876332005</v>
+      </c>
+    </row>
+    <row r="3738" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3738" s="9">
+        <v>42736</v>
+      </c>
+      <c r="B3738" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3738" s="3">
+        <v>9156.4286395324998</v>
+      </c>
+    </row>
+    <row r="3739" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3739" s="9">
+        <v>43101</v>
+      </c>
+      <c r="B3739" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3739" s="3">
+        <v>9173.7268183490305</v>
+      </c>
+    </row>
+    <row r="3740" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3740" s="9">
+        <v>43466</v>
+      </c>
+      <c r="B3740" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3740" s="3">
+        <v>9415.7213340026901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>